<commit_message>
feat(input): Ya no se requiere feature_nbr y todo se hace con feature_name
</commit_message>
<xml_diff>
--- a/data/sample-input.xlsx
+++ b/data/sample-input.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
   <si>
     <t>dept_nbr</t>
   </si>
@@ -39,9 +39,6 @@
     <t>max_feature_qty</t>
   </si>
   <si>
-    <t>feature_nbr</t>
-  </si>
-  <si>
     <t>feature_name</t>
   </si>
   <si>
@@ -94,9 +91,6 @@
   </si>
   <si>
     <t>Máximas piezas totales el el display</t>
-  </si>
-  <si>
-    <t>Número único del display</t>
   </si>
   <si>
     <t>Nombre único del display</t>
@@ -146,9 +140,6 @@
   </si>
   <si>
     <t>feature_name*</t>
-  </si>
-  <si>
-    <t>feature_nbr*</t>
   </si>
   <si>
     <t>dept_nbr*</t>
@@ -535,257 +526,235 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" customWidth="1"/>
-    <col min="8" max="8" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" customWidth="1"/>
+    <col min="7" max="7" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
       </c>
       <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+    </row>
+    <row r="2" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="4">
+        <v>95</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>9506783</v>
+      </c>
+      <c r="E2" s="4">
+        <v>3000</v>
+      </c>
+      <c r="F2" s="4">
+        <v>30</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="5">
+        <v>11840</v>
+      </c>
+      <c r="I2" s="5">
+        <v>11847</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="4">
+        <v>95</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4">
+        <v>9506804</v>
+      </c>
+      <c r="E3" s="4">
+        <v>3000</v>
+      </c>
+      <c r="F3" s="4">
+        <v>30</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="5">
+        <v>11840</v>
+      </c>
+      <c r="I3" s="5">
+        <v>11847</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>95</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>9574857</v>
+      </c>
+      <c r="E4">
+        <v>3000</v>
+      </c>
+      <c r="F4">
+        <v>30</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="1">
+        <v>11840</v>
+      </c>
+      <c r="I4" s="1">
+        <v>11847</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>95</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>9506748</v>
+      </c>
+      <c r="E5">
+        <v>3000</v>
+      </c>
+      <c r="F5">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="1">
+        <v>11840</v>
+      </c>
+      <c r="I5" s="1">
+        <v>11847</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>95</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>9574857</v>
+      </c>
+      <c r="E6">
+        <v>3000</v>
+      </c>
+      <c r="F6">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="H6" s="1">
+        <v>11902</v>
+      </c>
+      <c r="I6" s="1">
+        <v>11905</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="4">
+      <c r="B7">
         <v>95</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="C7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4">
-        <v>9506783</v>
-      </c>
-      <c r="F2" s="4">
+      <c r="D7">
+        <v>9506748</v>
+      </c>
+      <c r="E7">
         <v>3000</v>
       </c>
-      <c r="G2" s="4">
+      <c r="F7">
         <v>30</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="5">
-        <v>11840</v>
-      </c>
-      <c r="J2" s="5">
-        <v>11847</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="4">
-        <v>95</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="4">
-        <v>9506804</v>
-      </c>
-      <c r="F3" s="4">
-        <v>3000</v>
-      </c>
-      <c r="G3" s="4">
-        <v>30</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="5">
-        <v>11840</v>
-      </c>
-      <c r="J3" s="5">
-        <v>11847</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4">
-        <v>95</v>
-      </c>
-      <c r="D4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>9574857</v>
-      </c>
-      <c r="F4">
-        <v>3000</v>
-      </c>
-      <c r="G4">
-        <v>30</v>
-      </c>
-      <c r="H4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="1">
-        <v>11840</v>
-      </c>
-      <c r="J4" s="1">
-        <v>11847</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>1</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5">
-        <v>95</v>
-      </c>
-      <c r="D5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>9506748</v>
-      </c>
-      <c r="F5">
-        <v>3000</v>
-      </c>
-      <c r="G5">
-        <v>30</v>
-      </c>
-      <c r="H5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="1">
-        <v>11840</v>
-      </c>
-      <c r="J5" s="1">
-        <v>11847</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>2</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6">
-        <v>95</v>
-      </c>
-      <c r="D6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6">
-        <v>9574857</v>
-      </c>
-      <c r="F6">
-        <v>3000</v>
-      </c>
-      <c r="G6">
-        <v>30</v>
-      </c>
-      <c r="H6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="1">
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="1">
         <v>11902</v>
       </c>
-      <c r="J6" s="1">
+      <c r="I7" s="1">
         <v>11905</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>2</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7">
-        <v>95</v>
-      </c>
-      <c r="D7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <v>9506748</v>
-      </c>
-      <c r="F7">
-        <v>3000</v>
-      </c>
-      <c r="G7">
-        <v>30</v>
-      </c>
-      <c r="H7" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" s="1">
-        <v>11902</v>
-      </c>
-      <c r="J7" s="1">
-        <v>11905</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -795,10 +764,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -809,32 +778,32 @@
   <sheetData>
     <row r="1" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
@@ -842,7 +811,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
@@ -850,7 +819,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
         <v>21</v>
@@ -858,53 +827,50 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
-        <v>29</v>
+      <c r="A14" s="7" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -920,11 +886,6 @@
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>